<commit_message>
Added HW 1 Table screenshots
</commit_message>
<xml_diff>
--- a/HW 1/HW 1.xlsx
+++ b/HW 1/HW 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/228d21c66ed90b6a/Рабочий стол/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/228d21c66ed90b6a/Рабочий стол/GlobalLogicDevOpsBootCampv2/HW 1/HW 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="494" documentId="11_F25DC773A252ABDACC10480A61DB6DC65ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00E12B46-AD32-4196-A79C-9BA84383434C}"/>
@@ -320,9 +320,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -331,17 +331,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -357,7 +356,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -370,8 +369,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -462,13 +461,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -491,6 +483,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -540,8 +539,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15408B8C-3C71-4847-A310-C102E56C771E}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{15408B8C-3C71-4847-A310-C102E56C771E}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <autoFilter ref="A1:D14" xr:uid="{15408B8C-3C71-4847-A310-C102E56C771E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4422BBB4-09FA-46F5-A1C6-AA8791373DA2}" name="Name" dataDxfId="3"/>
@@ -816,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -832,498 +835,475 @@
     <col min="7" max="7" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>500</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>500</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="22" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>50</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="22" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>5</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="32.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="32.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>500</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" ht="22" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>1000</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="22" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>300</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>50</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>1</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="43" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="43" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>100</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="22" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>500</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>2</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>2000</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="32.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:4" ht="32.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>100</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="22" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>1000</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="16">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="15">
         <f>B2*C2+B3+B4*C4+B5*C5+B6*C6+B7*C7+B8*C8+B9*C9+B10*C10+B11*C11+B12*C12+B13+B14</f>
         <v>11680</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="16">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="15">
         <f>B4*12+B5*12+B13*12+B14*12</f>
         <v>13860</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="16">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="15">
         <f>D16+D15</f>
         <v>25540</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="22"/>
-      <c r="B24" s="21" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="22"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="20" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="22">
         <f>D16/12</f>
         <v>1155</v>
       </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="23">
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="22">
         <v>972</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="25">
         <f>D15</f>
         <v>11680</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26">
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25">
         <v>0</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B28" s="25">
         <f>D16</f>
         <v>13860</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26">
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25">
         <f>E26*12</f>
         <v>11664</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="26">
+      <c r="B29" s="25">
         <f>D17</f>
         <v>25540</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26">
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25">
         <f>E26*12</f>
         <v>11664</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="29">
         <f>B29-E29</f>
         <v>13876</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>